<commit_message>
add 312 & 121 & 122
</commit_message>
<xml_diff>
--- a/SmartLab寒假编程训练.xlsx
+++ b/SmartLab寒假编程训练.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>分类</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/burst-balloons/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-iii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-iv/</t>
   </si>
 </sst>
 </file>
@@ -819,8 +825,8 @@
   </sheetPr>
   <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1090,21 +1096,33 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
-      <c r="B22" s="16"/>
+      <c r="B22" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="C22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
-      <c r="B23" s="16"/>
+      <c r="B23" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="C23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="8"/>
+      <c r="D23" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
@@ -4956,8 +4974,12 @@
     <hyperlink ref="D21" r:id="rId14"/>
     <hyperlink ref="E19" r:id="rId15"/>
     <hyperlink ref="E21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18"/>
+    <hyperlink ref="E22" r:id="rId19"/>
+    <hyperlink ref="E23" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix 1036 & 122 && add 123 & 188
</commit_message>
<xml_diff>
--- a/SmartLab寒假编程训练.xlsx
+++ b/SmartLab寒假编程训练.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ClionProjects\MyLeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467C3F20-6F76-4108-BD76-34A2D8FED333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="算法题" sheetId="3" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>分类</t>
   </si>
@@ -291,12 +292,16 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock-iv/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/escape-a-large-maze/</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -819,14 +824,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1134,8 +1139,12 @@
       <c r="C24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
+      <c r="D24" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
@@ -4958,28 +4967,30 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
-    <hyperlink ref="E12" r:id="rId2"/>
-    <hyperlink ref="E13" r:id="rId3"/>
-    <hyperlink ref="D13" r:id="rId4"/>
-    <hyperlink ref="D16" r:id="rId5"/>
-    <hyperlink ref="E16" r:id="rId6"/>
-    <hyperlink ref="D20" r:id="rId7"/>
-    <hyperlink ref="E20" r:id="rId8"/>
-    <hyperlink ref="D33" r:id="rId9"/>
-    <hyperlink ref="D36" r:id="rId10"/>
-    <hyperlink ref="E33" r:id="rId11"/>
-    <hyperlink ref="E36" r:id="rId12"/>
-    <hyperlink ref="D19" r:id="rId13"/>
-    <hyperlink ref="D21" r:id="rId14"/>
-    <hyperlink ref="E19" r:id="rId15"/>
-    <hyperlink ref="E21" r:id="rId16"/>
-    <hyperlink ref="D22" r:id="rId17"/>
-    <hyperlink ref="D23" r:id="rId18"/>
-    <hyperlink ref="E22" r:id="rId19"/>
-    <hyperlink ref="E23" r:id="rId20"/>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E33" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E36" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D24" r:id="rId21" xr:uid="{9B2AABB1-530E-4F99-AB6D-BDF532B30F82}"/>
+    <hyperlink ref="E24" r:id="rId22" xr:uid="{2353A1A6-B595-49F2-A646-8F64F08F2787}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 382 & 398
</commit_message>
<xml_diff>
--- a/SmartLab寒假编程训练.xlsx
+++ b/SmartLab寒假编程训练.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ClionProjects\MyLeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5919A5-9678-4E53-A664-DF2EB478CED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B852A45-38E0-4866-BDFF-1E6E6A2BA3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
   <si>
     <t>分类</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/all-oone-data-structure/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/random-pick-index/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-random-node/</t>
   </si>
 </sst>
 </file>
@@ -846,8 +852,8 @@
   </sheetPr>
   <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1188,8 +1194,12 @@
       <c r="C25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
+      <c r="D25" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
@@ -1199,8 +1209,12 @@
       <c r="C26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="8"/>
+      <c r="D26" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
@@ -5033,8 +5047,12 @@
     <hyperlink ref="E17" r:id="rId28" xr:uid="{9EC4A49A-1C29-40D2-8E3B-050E35AA031A}"/>
     <hyperlink ref="D14" r:id="rId29" xr:uid="{4063CB27-CC98-4CCF-A08C-F616CB99B2CD}"/>
     <hyperlink ref="E14" r:id="rId30" xr:uid="{BBC560ED-8D63-4612-9E91-118A36A127B3}"/>
+    <hyperlink ref="D26" r:id="rId31" xr:uid="{395644BA-8EA3-4E06-9213-9798359B2023}"/>
+    <hyperlink ref="D25" r:id="rId32" xr:uid="{92EFAD95-3BD1-4A58-B057-4F1AE2B4F89D}"/>
+    <hyperlink ref="E25" r:id="rId33" xr:uid="{E76D1087-ED6C-44B0-B0F0-B3CA075C1EE7}"/>
+    <hyperlink ref="E26" r:id="rId34" xr:uid="{13213FAF-EE94-485A-89DD-9E5E4999006A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 56 & 295 & 547
</commit_message>
<xml_diff>
--- a/SmartLab寒假编程训练.xlsx
+++ b/SmartLab寒假编程训练.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ClionProjects\MyLeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B852A45-38E0-4866-BDFF-1E6E6A2BA3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C9C1D5-837E-4B41-9DBE-D042614D5956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
   <si>
     <t>分类</t>
   </si>
@@ -318,6 +318,30 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/linked-list-random-node/</t>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-intervals/</t>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-median-from-data-stream/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/friend-circles/</t>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/range-sum-query-immutable/</t>
   </si>
 </sst>
 </file>
@@ -852,8 +876,8 @@
   </sheetPr>
   <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1220,44 +1244,66 @@
       <c r="A27" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="C27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
+      <c r="D27" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="C28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
+      <c r="D28" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="C29" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
+      <c r="D29" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="16"/>
+      <c r="B30" s="16" t="s">
+        <v>85</v>
+      </c>
       <c r="C30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="D30" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5025,34 +5071,41 @@
     <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="D20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="E20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E33" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E36" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D24" r:id="rId21" xr:uid="{9B2AABB1-530E-4F99-AB6D-BDF532B30F82}"/>
-    <hyperlink ref="E24" r:id="rId22" xr:uid="{2353A1A6-B595-49F2-A646-8F64F08F2787}"/>
-    <hyperlink ref="D18" r:id="rId23" xr:uid="{55D02DAB-BE0E-4934-A1CE-A0327E57CCCF}"/>
-    <hyperlink ref="E18" r:id="rId24" xr:uid="{1955DA69-CC59-47CD-B99D-1825BC5D883B}"/>
-    <hyperlink ref="D15" r:id="rId25" xr:uid="{45FC9469-17B6-452C-876A-A2C5CE3832A3}"/>
-    <hyperlink ref="E15" r:id="rId26" xr:uid="{D83C779E-28B2-4DBF-8863-411AC8EE5D0A}"/>
-    <hyperlink ref="D17" r:id="rId27" xr:uid="{5D1910CA-4BF9-4ADF-BE90-6CBD659446C0}"/>
-    <hyperlink ref="E17" r:id="rId28" xr:uid="{9EC4A49A-1C29-40D2-8E3B-050E35AA031A}"/>
-    <hyperlink ref="D14" r:id="rId29" xr:uid="{4063CB27-CC98-4CCF-A08C-F616CB99B2CD}"/>
-    <hyperlink ref="E14" r:id="rId30" xr:uid="{BBC560ED-8D63-4612-9E91-118A36A127B3}"/>
-    <hyperlink ref="D26" r:id="rId31" xr:uid="{395644BA-8EA3-4E06-9213-9798359B2023}"/>
-    <hyperlink ref="D25" r:id="rId32" xr:uid="{92EFAD95-3BD1-4A58-B057-4F1AE2B4F89D}"/>
-    <hyperlink ref="E25" r:id="rId33" xr:uid="{E76D1087-ED6C-44B0-B0F0-B3CA075C1EE7}"/>
-    <hyperlink ref="E26" r:id="rId34" xr:uid="{13213FAF-EE94-485A-89DD-9E5E4999006A}"/>
+    <hyperlink ref="E33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D21" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D22" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D23" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D24" r:id="rId19" xr:uid="{9B2AABB1-530E-4F99-AB6D-BDF532B30F82}"/>
+    <hyperlink ref="E24" r:id="rId20" xr:uid="{2353A1A6-B595-49F2-A646-8F64F08F2787}"/>
+    <hyperlink ref="D18" r:id="rId21" xr:uid="{55D02DAB-BE0E-4934-A1CE-A0327E57CCCF}"/>
+    <hyperlink ref="E18" r:id="rId22" xr:uid="{1955DA69-CC59-47CD-B99D-1825BC5D883B}"/>
+    <hyperlink ref="D15" r:id="rId23" xr:uid="{45FC9469-17B6-452C-876A-A2C5CE3832A3}"/>
+    <hyperlink ref="E15" r:id="rId24" xr:uid="{D83C779E-28B2-4DBF-8863-411AC8EE5D0A}"/>
+    <hyperlink ref="D17" r:id="rId25" xr:uid="{5D1910CA-4BF9-4ADF-BE90-6CBD659446C0}"/>
+    <hyperlink ref="E17" r:id="rId26" xr:uid="{9EC4A49A-1C29-40D2-8E3B-050E35AA031A}"/>
+    <hyperlink ref="D14" r:id="rId27" xr:uid="{4063CB27-CC98-4CCF-A08C-F616CB99B2CD}"/>
+    <hyperlink ref="E14" r:id="rId28" xr:uid="{BBC560ED-8D63-4612-9E91-118A36A127B3}"/>
+    <hyperlink ref="D26" r:id="rId29" xr:uid="{395644BA-8EA3-4E06-9213-9798359B2023}"/>
+    <hyperlink ref="D25" r:id="rId30" xr:uid="{92EFAD95-3BD1-4A58-B057-4F1AE2B4F89D}"/>
+    <hyperlink ref="E25" r:id="rId31" xr:uid="{E76D1087-ED6C-44B0-B0F0-B3CA075C1EE7}"/>
+    <hyperlink ref="E26" r:id="rId32" xr:uid="{13213FAF-EE94-485A-89DD-9E5E4999006A}"/>
+    <hyperlink ref="D27" r:id="rId33" xr:uid="{97E6B46C-50AE-4174-8944-5C8E1B276093}"/>
+    <hyperlink ref="E27" r:id="rId34" xr:uid="{1204CF59-2C46-4CDD-B79F-C259087D56A6}"/>
+    <hyperlink ref="D36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D33" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D28" r:id="rId37" xr:uid="{C5C7AC9E-F24B-48E3-B9E4-FDA4BBA244CF}"/>
+    <hyperlink ref="E28" r:id="rId38" xr:uid="{12E574DD-0E66-45B9-9DF4-6F15603546DA}"/>
+    <hyperlink ref="D29" r:id="rId39" xr:uid="{9F101B68-027B-4C32-8B4D-7F1FC55ECC4D}"/>
+    <hyperlink ref="E29" r:id="rId40" xr:uid="{002FFDF5-1EE5-4C94-A78D-75EB30187544}"/>
+    <hyperlink ref="D30" r:id="rId41" xr:uid="{21F667C2-98E5-4C5E-B8CB-D22EC4073561}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 303 & 307
</commit_message>
<xml_diff>
--- a/SmartLab寒假编程训练.xlsx
+++ b/SmartLab寒假编程训练.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ClionProjects\MyLeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C9C1D5-837E-4B41-9DBE-D042614D5956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F216AC-5D45-4F4F-8EC7-BEC0A192FCFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
   <si>
     <t>分类</t>
   </si>
@@ -342,6 +342,13 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/range-sum-query-immutable/</t>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/range-sum-query-mutable/</t>
   </si>
 </sst>
 </file>
@@ -876,8 +883,8 @@
   </sheetPr>
   <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1304,16 +1311,24 @@
       <c r="D30" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="22"/>
-      <c r="B31" s="16"/>
+      <c r="B31" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="8"/>
+      <c r="D31" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23"/>
@@ -1322,7 +1337,7 @@
         <v>46</v>
       </c>
       <c r="D32" s="11"/>
-      <c r="E32" s="8"/>
+      <c r="E32" s="19"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="21" t="s">
@@ -5104,8 +5119,11 @@
     <hyperlink ref="D29" r:id="rId39" xr:uid="{9F101B68-027B-4C32-8B4D-7F1FC55ECC4D}"/>
     <hyperlink ref="E29" r:id="rId40" xr:uid="{002FFDF5-1EE5-4C94-A78D-75EB30187544}"/>
     <hyperlink ref="D30" r:id="rId41" xr:uid="{21F667C2-98E5-4C5E-B8CB-D22EC4073561}"/>
+    <hyperlink ref="E30" r:id="rId42" xr:uid="{D0BEC808-10B9-4072-BE01-E776DDC4397F}"/>
+    <hyperlink ref="E31" r:id="rId43" xr:uid="{5E6E1DF9-BA1E-4559-BBF5-E5BC1C38BE9D}"/>
+    <hyperlink ref="D31" r:id="rId44" xr:uid="{1599C469-3AC1-4719-9740-804A8DC2ACF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 410 & 416 & 630
</commit_message>
<xml_diff>
--- a/SmartLab寒假编程训练.xlsx
+++ b/SmartLab寒假编程训练.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ClionProjects\MyLeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC46DEE-F339-4F02-9B77-961FE2AD1499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2769C128-E467-4573-9CC3-F2ACC8EF21D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>分类</t>
   </si>
@@ -591,6 +591,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -601,8 +603,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -923,8 +923,8 @@
   </sheetPr>
   <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -967,7 +967,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="15"/>
@@ -979,7 +979,7 @@
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="15"/>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -989,7 +989,7 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="15"/>
       <c r="C6" s="6" t="s">
         <v>57</v>
@@ -999,7 +999,7 @@
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="15"/>
       <c r="C7" s="6" t="s">
         <v>58</v>
@@ -1009,7 +1009,7 @@
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="15"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
@@ -1019,7 +1019,7 @@
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="15"/>
       <c r="C9" s="6" t="s">
         <v>12</v>
@@ -1029,22 +1029,22 @@
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="15"/>
       <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="8"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="15"/>
       <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="8"/>
       <c r="F11" s="12"/>
     </row>
@@ -1067,7 +1067,7 @@
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="22"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="15" t="s">
         <v>19</v>
       </c>
@@ -1099,7 +1099,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1116,7 +1116,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="22"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="15" t="s">
         <v>16</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="22"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
@@ -1147,7 +1147,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="15" t="s">
         <v>19</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -1179,7 +1179,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="22"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="15" t="s">
         <v>16</v>
       </c>
@@ -1194,7 +1194,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
@@ -1209,7 +1209,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="15" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="22"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="15" t="s">
         <v>19</v>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="15" t="s">
         <v>73</v>
       </c>
@@ -1339,7 +1339,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="20"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="15" t="s">
         <v>87</v>
       </c>
@@ -1371,7 +1371,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="15" t="s">
         <v>89</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="15" t="s">
@@ -1403,7 +1403,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="15" t="s">
         <v>91</v>
       </c>
@@ -1418,7 +1418,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="15" t="s">
         <v>89</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="15" t="s">
@@ -1450,7 +1450,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="15" t="s">
         <v>91</v>
       </c>
@@ -1460,10 +1460,12 @@
       <c r="D37" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="21"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="15" t="s">
         <v>89</v>
       </c>
@@ -1473,7 +1475,9 @@
       <c r="D38" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B39" s="16"/>
@@ -5196,8 +5200,10 @@
     <hyperlink ref="D38" r:id="rId50" xr:uid="{7308551A-6473-4598-8C92-60D5DFFA7C82}"/>
     <hyperlink ref="E34" r:id="rId51" xr:uid="{91220D72-C127-494A-A95F-1378281ED5D7}"/>
     <hyperlink ref="E35" r:id="rId52" xr:uid="{2FF7A6D0-69D9-4F96-95B4-D114DC3C2EC1}"/>
+    <hyperlink ref="E37" r:id="rId53" xr:uid="{D3132CCE-B930-4F79-B389-56350DF6AD20}"/>
+    <hyperlink ref="E38" r:id="rId54" xr:uid="{DC384904-BC9B-4FE2-998B-0986D5C8DA1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>